<commit_message>
Allow datetime objects in info dict
</commit_message>
<xml_diff>
--- a/tests/sample_data/neware/Experiment_Record.xlsx
+++ b/tests/sample_data/neware/Experiment_Record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/GitHub/PyBatDATA/tests/sample_data_neware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/GitHub/personal/PyProBE/tests/sample_data/neware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E224D-1860-8549-A689-04CACB515DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0CA4D6-B39D-8440-A9DD-75D5C857A929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="22880" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
   <si>
     <t>Test_Cell</t>
+  </si>
+  <si>
+    <t>Test Date</t>
   </si>
 </sst>
 </file>
@@ -66,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,22 +352,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: remove colour generation in make_cell_list method
</commit_message>
<xml_diff>
--- a/tests/sample_data/neware/Experiment_Record.xlsx
+++ b/tests/sample_data/neware/Experiment_Record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/GitHub/PyBatDATA/tests/sample_data_neware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/GitHub/personal/PyProBE/tests/sample_data/neware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E224D-1860-8549-A689-04CACB515DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA33ED6D-FFEA-DD4D-B6CC-77AF2F4D70B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="760" windowWidth="22880" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Test_Cell</t>
+    <t>Cell2</t>
+  </si>
+  <si>
+    <t>Cell3</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>NMC622</t>
+  </si>
+  <si>
+    <t>LFP</t>
+  </si>
+  <si>
+    <t>Nominal Capacity [Ah]</t>
+  </si>
+  <si>
+    <t>Cell1</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>NMC811</t>
   </si>
 </sst>
 </file>
@@ -66,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,25 +373,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45371.377349537041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45371.376655092594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45371.377349537041</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>